<commit_message>
changes to data an dcode
</commit_message>
<xml_diff>
--- a/Q_oscillator/data/Q_oscillator_data.xlsx
+++ b/Q_oscillator/data/Q_oscillator_data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29415"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julianwoo/Library/Mobile Documents/com~apple~CloudDocs/PHY324/PHY324_Experiment/Q_oscillator/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bd6b3ef14d80b5b/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0F5E8A-9F09-A84F-ACDE-C35CC1BF33B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABC93CED-93CC-4ADC-9D75-6179BF9D1527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31180" yWindow="2560" windowWidth="20020" windowHeight="17440" activeTab="1" xr2:uid="{568F41B4-D0EF-7E4F-A74D-1B74E3ACBC6A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="28800" firstSheet="3" activeTab="3" xr2:uid="{568F41B4-D0EF-7E4F-A74D-1B74E3ACBC6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Ex1" sheetId="1" r:id="rId1"/>
     <sheet name="Ex2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Sin Frequency (KHz)</t>
   </si>
@@ -46,7 +47,13 @@
     <t xml:space="preserve"> Input voltage (V)</t>
   </si>
   <si>
+    <t>input uncertainty</t>
+  </si>
+  <si>
     <t>Output  Voltage (V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Output uncertainty</t>
   </si>
   <si>
     <t>V_r / v_in</t>
@@ -58,40 +65,40 @@
     <t>phase uncertainty</t>
   </si>
   <si>
-    <t xml:space="preserve"> Output uncertainty</t>
-  </si>
-  <si>
-    <t>input uncertainty</t>
-  </si>
-  <si>
     <t>mean voltage (v)</t>
   </si>
   <si>
     <t>uncertainty</t>
   </si>
   <si>
-    <t>output</t>
+    <t>input volt v</t>
+  </si>
+  <si>
+    <t>output v</t>
   </si>
   <si>
     <t>phase</t>
   </si>
   <si>
-    <t>output v</t>
+    <t>avg</t>
   </si>
   <si>
-    <t>input volt v</t>
+    <t>pointed 45</t>
   </si>
   <si>
     <t>1.45 +0.5</t>
   </si>
   <si>
-    <t>avg</t>
+    <t>0.3 mh</t>
+  </si>
+  <si>
+    <t>87.8 ohms</t>
+  </si>
+  <si>
+    <t>1.3-4</t>
   </si>
   <si>
     <t>1.3-2.4</t>
-  </si>
-  <si>
-    <t>1.3-4</t>
   </si>
   <si>
     <t>0.3-1</t>
@@ -100,19 +107,10 @@
     <t>0.703-705</t>
   </si>
   <si>
-    <t>pointed 45</t>
-  </si>
-  <si>
-    <t>0.3 mh</t>
-  </si>
-  <si>
-    <t>87.8 ohms</t>
+    <t>3.159 mh</t>
   </si>
   <si>
     <t>0.03 nf</t>
-  </si>
-  <si>
-    <t>3.159 mh</t>
   </si>
   <si>
     <t>400khz</t>
@@ -145,10 +143,49 @@
     <t>input</t>
   </si>
   <si>
+    <t>output</t>
+  </si>
+  <si>
     <t>phase radians</t>
   </si>
   <si>
     <t>ratio</t>
+  </si>
+  <si>
+    <t>freq (Khz)</t>
+  </si>
+  <si>
+    <t>freq unc</t>
+  </si>
+  <si>
+    <t>input unc</t>
+  </si>
+  <si>
+    <t>output mv</t>
+  </si>
+  <si>
+    <t>phase (deg)</t>
+  </si>
+  <si>
+    <t>input div (V)</t>
+  </si>
+  <si>
+    <t>output div (V)</t>
+  </si>
+  <si>
+    <t>capacitance</t>
+  </si>
+  <si>
+    <t>inductance</t>
+  </si>
+  <si>
+    <t>0.01  nf</t>
+  </si>
+  <si>
+    <t>113.9 mh</t>
+  </si>
+  <si>
+    <t>0.29 nf</t>
   </si>
 </sst>
 </file>
@@ -162,7 +199,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +212,13 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -198,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -207,6 +251,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,9 +592,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,25 +602,25 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0.40039999999999998</v>
       </c>
@@ -606,7 +651,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>0.80030000000000001</v>
       </c>
@@ -637,7 +682,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1.1979</v>
       </c>
@@ -667,7 +712,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1.5992999999999999</v>
       </c>
@@ -697,7 +742,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>2.0009999999999999</v>
       </c>
@@ -727,7 +772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>2.399</v>
       </c>
@@ -757,7 +802,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>2.7989999999999999</v>
       </c>
@@ -787,7 +832,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="2">
         <v>3.2</v>
       </c>
@@ -817,7 +862,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>3.5990000000000002</v>
       </c>
@@ -847,7 +892,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="2">
         <v>4</v>
       </c>
@@ -877,7 +922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="2">
         <v>4.4039999999999999</v>
       </c>
@@ -907,7 +952,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="2">
         <v>4.75</v>
       </c>
@@ -937,7 +982,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="2">
         <v>4.7729999999999997</v>
       </c>
@@ -967,7 +1012,7 @@
         <v>4.7750000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="2">
         <v>4.806</v>
       </c>
@@ -997,7 +1042,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="2">
         <v>4.8259999999999996</v>
       </c>
@@ -1027,7 +1072,7 @@
         <v>4.8250000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="2">
         <v>4.8490000000000002</v>
       </c>
@@ -1057,7 +1102,7 @@
         <v>4.8499999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="2">
         <v>4.875</v>
       </c>
@@ -1087,7 +1132,7 @@
         <v>4.875</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="2">
         <v>4.9000000000000004</v>
       </c>
@@ -1117,7 +1162,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="2">
         <v>4.9249999999999998</v>
       </c>
@@ -1147,7 +1192,7 @@
         <v>4.9249999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="2">
         <v>4.95</v>
       </c>
@@ -1177,7 +1222,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="2">
         <v>4.9740000000000002</v>
       </c>
@@ -1207,7 +1252,7 @@
         <v>4.9749999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="2">
         <v>5</v>
       </c>
@@ -1237,7 +1282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="2">
         <v>5.2030000000000003</v>
       </c>
@@ -1267,7 +1312,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="2">
         <v>5.6059999999999999</v>
       </c>
@@ -1297,7 +1342,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="2">
         <v>6</v>
       </c>
@@ -1327,64 +1372,64 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="2"/>
     </row>
   </sheetData>
@@ -1396,13 +1441,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90B7C2D-8280-6745-AE8C-8FD9DE525505}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1413,23 +1458,23 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="4">
         <v>10</v>
       </c>
@@ -1449,19 +1494,19 @@
         <v>3.589</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>0.57562000000000002</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="4">
         <v>12.5</v>
       </c>
@@ -1481,13 +1526,13 @@
         <v>3.59</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3">
         <v>0.60238999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="4">
         <v>15</v>
       </c>
@@ -1507,13 +1552,13 @@
         <v>3.5979999999999999</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H4">
         <v>0.63580000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="4">
         <v>17.5</v>
       </c>
@@ -1533,13 +1578,13 @@
         <v>3.5880000000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H5">
         <v>0.67588999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="4">
         <v>20</v>
       </c>
@@ -1559,10 +1604,10 @@
         <v>3.5880000000000001</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="4">
         <v>22.5</v>
       </c>
@@ -1585,7 +1630,7 @@
         <v>0.54905000000000004</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M7" t="s">
         <v>23</v>
@@ -1594,7 +1639,7 @@
         <v>224.5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="4">
         <v>25</v>
       </c>
@@ -1617,7 +1662,7 @@
         <v>0.52232999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="4">
         <v>27.5</v>
       </c>
@@ -1640,7 +1685,7 @@
         <v>0.51571999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="6">
         <v>30</v>
       </c>
@@ -1663,7 +1708,7 @@
         <v>0.51346999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="6">
         <v>32.5</v>
       </c>
@@ -1686,7 +1731,7 @@
         <v>0.51349199999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" s="6">
         <v>35</v>
       </c>
@@ -1709,7 +1754,7 @@
         <v>0.51826000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="6">
         <v>37.5</v>
       </c>
@@ -1732,7 +1777,7 @@
         <v>0.52264999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" s="6">
         <v>40</v>
       </c>
@@ -1755,7 +1800,7 @@
         <v>0.52637999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" s="6">
         <v>42.5</v>
       </c>
@@ -1778,7 +1823,7 @@
         <v>0.52968999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" s="6">
         <v>43</v>
       </c>
@@ -1801,7 +1846,7 @@
         <v>0.53205000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16">
       <c r="A17" s="6">
         <v>43.35</v>
       </c>
@@ -1824,7 +1869,7 @@
         <v>0.53444999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16">
       <c r="A18" s="6">
         <v>43.4</v>
       </c>
@@ -1847,7 +1892,7 @@
         <v>0.53676000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16">
       <c r="A19" s="6">
         <v>43.45</v>
       </c>
@@ -1870,7 +1915,7 @@
         <v>0.54744999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16">
       <c r="A20" s="6">
         <v>43.5</v>
       </c>
@@ -1893,7 +1938,7 @@
         <v>0.54193000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16">
       <c r="A21" s="6">
         <v>43.55</v>
       </c>
@@ -1916,7 +1961,7 @@
         <v>0.55054000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16">
       <c r="A22" s="6">
         <v>43.6</v>
       </c>
@@ -1939,7 +1984,7 @@
         <v>0.55388999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16">
       <c r="A23" s="6">
         <v>43.65</v>
       </c>
@@ -1968,7 +2013,7 @@
         <v>3.9148999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16">
       <c r="A24" s="6">
         <v>47.5</v>
       </c>
@@ -2003,7 +2048,7 @@
         <v>0.90164999999999995</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16">
       <c r="A25" s="6">
         <v>50</v>
       </c>
@@ -2044,7 +2089,7 @@
         <v>3.9163999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16">
       <c r="C26" s="2"/>
       <c r="K26">
         <v>200</v>
@@ -2062,7 +2107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16">
       <c r="A27" s="6"/>
       <c r="C27" s="2"/>
       <c r="K27">
@@ -2078,7 +2123,7 @@
         <v>0.89105000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16">
       <c r="K28">
         <v>300</v>
       </c>
@@ -2092,9 +2137,9 @@
         <v>0.99670000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K29">
         <v>350</v>
@@ -2109,7 +2154,7 @@
         <v>0.78705999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16">
       <c r="A30" s="6"/>
       <c r="C30" s="3"/>
       <c r="K30">
@@ -2125,7 +2170,7 @@
         <v>0.77429999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16">
       <c r="A31" s="6"/>
       <c r="C31" s="3"/>
       <c r="K31">
@@ -2141,7 +2186,7 @@
         <v>0.80498999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16">
       <c r="A32" s="6"/>
       <c r="C32" s="3"/>
       <c r="K32">
@@ -2157,7 +2202,7 @@
         <v>0.83021</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14">
       <c r="A33" s="6"/>
       <c r="C33" s="3"/>
       <c r="K33">
@@ -2173,7 +2218,7 @@
         <v>0.84672000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14">
       <c r="A34" s="6"/>
       <c r="C34" s="3"/>
       <c r="K34">
@@ -2189,7 +2234,7 @@
         <v>0.85836999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14">
       <c r="A35" s="4"/>
       <c r="C35" s="3"/>
       <c r="K35">
@@ -2205,7 +2250,7 @@
         <v>0.89410999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14">
       <c r="A36" s="4"/>
       <c r="C36" s="7"/>
       <c r="K36">
@@ -2221,7 +2266,7 @@
         <v>0.89902000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14">
       <c r="A37" s="4"/>
       <c r="C37" s="7"/>
       <c r="K37">
@@ -2237,7 +2282,7 @@
         <v>0.90488999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14">
       <c r="A38" s="4"/>
       <c r="C38" s="7"/>
       <c r="K38">
@@ -2253,7 +2298,7 @@
         <v>0.91022999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14">
       <c r="A39" s="4"/>
       <c r="C39" s="7"/>
       <c r="K39">
@@ -2269,11 +2314,11 @@
         <v>0.91751000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14">
       <c r="A40" s="4"/>
       <c r="C40" s="7"/>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E40">
         <v>3.9451000000000001</v>
@@ -2300,11 +2345,11 @@
         <v>0.91601999999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14">
       <c r="A41" s="4"/>
       <c r="C41" s="7"/>
       <c r="D41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E41">
         <v>3.9449999999999998</v>
@@ -2331,11 +2376,11 @@
         <v>0.91622000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14">
       <c r="A42" s="4"/>
       <c r="C42" s="7"/>
       <c r="D42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E42">
         <v>3.9453</v>
@@ -2362,7 +2407,7 @@
         <v>0.91542999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14">
       <c r="A43" s="4"/>
       <c r="C43" s="7"/>
       <c r="K43">
@@ -2378,7 +2423,7 @@
         <v>0.91064000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14">
       <c r="A44" s="4"/>
       <c r="C44" s="7"/>
       <c r="K44">
@@ -2394,7 +2439,7 @@
         <v>0.90941000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14">
       <c r="A45" s="4"/>
       <c r="C45" s="7"/>
       <c r="K45">
@@ -2410,7 +2455,7 @@
         <v>0.90781000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14">
       <c r="K46">
         <v>513.5</v>
       </c>
@@ -2424,7 +2469,7 @@
         <v>0.90536000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14">
       <c r="K47">
         <v>514</v>
       </c>
@@ -2438,7 +2483,7 @@
         <v>0.90176000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14">
       <c r="K48">
         <v>514.5</v>
       </c>
@@ -2452,7 +2497,7 @@
         <v>0.90027999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14">
       <c r="K49">
         <v>515</v>
       </c>
@@ -2466,7 +2511,7 @@
         <v>0.90112000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14">
       <c r="K50">
         <v>515.5</v>
       </c>
@@ -2480,7 +2525,7 @@
         <v>0.90083999999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14">
       <c r="K51">
         <v>516</v>
       </c>
@@ -2494,7 +2539,7 @@
         <v>0.90046999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14">
       <c r="K52">
         <v>516.5</v>
       </c>
@@ -2508,7 +2553,7 @@
         <v>0.90000999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14">
       <c r="K53">
         <v>517</v>
       </c>
@@ -2522,9 +2567,9 @@
         <v>0.90012000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K54">
         <v>517.5</v>
@@ -2539,7 +2584,7 @@
         <v>0.89953000000000005</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14">
       <c r="K55">
         <v>518</v>
       </c>
@@ -2553,7 +2598,7 @@
         <v>0.89756000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14">
       <c r="K56">
         <v>518.5</v>
       </c>
@@ -2567,7 +2612,7 @@
         <v>0.89692000000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14">
       <c r="K57">
         <v>519</v>
       </c>
@@ -2581,7 +2626,7 @@
         <v>0.89273999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14">
       <c r="K58">
         <v>519.5</v>
       </c>
@@ -2595,7 +2640,7 @@
         <v>0.89139000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14">
       <c r="K59">
         <v>520</v>
       </c>
@@ -2609,7 +2654,7 @@
         <v>0.88961000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14">
       <c r="K60">
         <v>530</v>
       </c>
@@ -2623,7 +2668,7 @@
         <v>0.88100999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14">
       <c r="K61">
         <v>540</v>
       </c>
@@ -2637,7 +2682,7 @@
         <v>0.86670999999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14">
       <c r="K62">
         <v>550</v>
       </c>
@@ -2651,7 +2696,7 @@
         <v>0.85370000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14">
       <c r="K63">
         <v>560</v>
       </c>
@@ -2665,7 +2710,7 @@
         <v>0.83816999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14">
       <c r="K64">
         <v>570</v>
       </c>
@@ -2679,7 +2724,7 @@
         <v>0.82765999999999995</v>
       </c>
     </row>
-    <row r="65" spans="11:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="11:16">
       <c r="K65">
         <v>580</v>
       </c>
@@ -2693,10 +2738,10 @@
         <v>0.81459000000000004</v>
       </c>
       <c r="P65" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="11:16" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="11:16">
       <c r="K66">
         <v>590</v>
       </c>
@@ -2710,7 +2755,7 @@
         <v>0.80322000000000005</v>
       </c>
     </row>
-    <row r="67" spans="11:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="11:16">
       <c r="K67">
         <v>600</v>
       </c>
@@ -2730,7 +2775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="11:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="11:16">
       <c r="K68">
         <v>700</v>
       </c>
@@ -2744,7 +2789,7 @@
         <v>0.77420999999999995</v>
       </c>
     </row>
-    <row r="69" spans="11:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="11:16">
       <c r="K69">
         <v>800</v>
       </c>
@@ -2758,7 +2803,7 @@
         <v>0.76176999999999995</v>
       </c>
     </row>
-    <row r="70" spans="11:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="11:16">
       <c r="K70">
         <v>900</v>
       </c>
@@ -2772,7 +2817,7 @@
         <v>0.75244999999999995</v>
       </c>
     </row>
-    <row r="71" spans="11:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="11:16">
       <c r="K71">
         <v>1000</v>
       </c>
@@ -2786,7 +2831,7 @@
         <v>0.74189000000000005</v>
       </c>
     </row>
-    <row r="72" spans="11:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="11:16">
       <c r="K72">
         <v>1500</v>
       </c>
@@ -2800,13 +2845,13 @@
         <v>0.73053999999999997</v>
       </c>
       <c r="O72" t="s">
+        <v>30</v>
+      </c>
+      <c r="P72" t="s">
         <v>31</v>
       </c>
-      <c r="P72" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="73" spans="11:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="11:16">
       <c r="K73">
         <v>2000</v>
       </c>
@@ -2820,9 +2865,9 @@
         <v>0.69059999999999999</v>
       </c>
     </row>
-    <row r="79" spans="11:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="11:16">
       <c r="K79" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L79">
         <v>3.9384000000000001</v>
@@ -2834,7 +2879,7 @@
         <v>0.96404999999999996</v>
       </c>
     </row>
-    <row r="80" spans="11:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="11:16">
       <c r="K80">
         <v>410</v>
       </c>
@@ -2848,7 +2893,7 @@
         <v>0.96501999999999999</v>
       </c>
     </row>
-    <row r="81" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="11:15">
       <c r="K81">
         <v>420</v>
       </c>
@@ -2862,7 +2907,7 @@
         <v>0.96599999999999997</v>
       </c>
     </row>
-    <row r="82" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="82" spans="11:15">
       <c r="K82">
         <v>430</v>
       </c>
@@ -2879,7 +2924,7 @@
         <v>0.96708000000000005</v>
       </c>
     </row>
-    <row r="83" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="83" spans="11:15">
       <c r="K83">
         <v>440</v>
       </c>
@@ -2893,7 +2938,7 @@
         <v>1.0828</v>
       </c>
     </row>
-    <row r="87" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="87" spans="11:15">
       <c r="K87">
         <v>480</v>
       </c>
@@ -2910,7 +2955,7 @@
         <v>1.0136000000000001</v>
       </c>
     </row>
-    <row r="88" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="88" spans="11:15">
       <c r="K88">
         <v>490</v>
       </c>
@@ -2927,7 +2972,7 @@
         <v>1.0238</v>
       </c>
     </row>
-    <row r="89" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="89" spans="11:15">
       <c r="K89">
         <v>495</v>
       </c>
@@ -2941,7 +2986,7 @@
         <v>0.96414999999999995</v>
       </c>
     </row>
-    <row r="90" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="90" spans="11:15">
       <c r="K90">
         <v>500</v>
       </c>
@@ -2955,7 +3000,7 @@
         <v>0.96543999999999996</v>
       </c>
     </row>
-    <row r="91" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="91" spans="11:15">
       <c r="K91">
         <v>505</v>
       </c>
@@ -2969,7 +3014,7 @@
         <v>0.96638999999999997</v>
       </c>
     </row>
-    <row r="92" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="92" spans="11:15">
       <c r="K92">
         <v>506</v>
       </c>
@@ -2983,7 +3028,7 @@
         <v>0.96753</v>
       </c>
     </row>
-    <row r="93" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="93" spans="11:15">
       <c r="K93">
         <v>507</v>
       </c>
@@ -2997,7 +3042,7 @@
         <v>0.96816999999999998</v>
       </c>
     </row>
-    <row r="94" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="94" spans="11:15">
       <c r="K94">
         <v>508</v>
       </c>
@@ -3011,7 +3056,7 @@
         <v>0.96994999999999998</v>
       </c>
     </row>
-    <row r="95" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="95" spans="11:15">
       <c r="K95">
         <v>509</v>
       </c>
@@ -3025,7 +3070,7 @@
         <v>0.97155000000000002</v>
       </c>
     </row>
-    <row r="96" spans="11:15" x14ac:dyDescent="0.2">
+    <row r="96" spans="11:15">
       <c r="K96">
         <v>510</v>
       </c>
@@ -3039,7 +3084,7 @@
         <v>0.97211000000000003</v>
       </c>
     </row>
-    <row r="97" spans="11:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="11:14">
       <c r="K97">
         <v>480</v>
       </c>
@@ -3053,7 +3098,7 @@
         <v>1.0445</v>
       </c>
     </row>
-    <row r="98" spans="11:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="11:14">
       <c r="K98">
         <v>490</v>
       </c>
@@ -3077,20 +3122,20 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>35</v>
@@ -3099,7 +3144,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>100</v>
       </c>
@@ -3117,7 +3162,7 @@
         <v>0.9988572879634332</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>150</v>
       </c>
@@ -3135,7 +3180,7 @@
         <v>0.99860360017264582</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>200</v>
       </c>
@@ -3149,7 +3194,7 @@
         <v>0.89219999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>250</v>
       </c>
@@ -3163,7 +3208,7 @@
         <v>0.89105000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>300</v>
       </c>
@@ -3177,7 +3222,7 @@
         <v>0.99670000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>350</v>
       </c>
@@ -3191,7 +3236,7 @@
         <v>0.78705999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>400</v>
       </c>
@@ -3205,7 +3250,7 @@
         <v>0.77429999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>450</v>
       </c>
@@ -3219,7 +3264,7 @@
         <v>0.80498999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>500</v>
       </c>
@@ -3233,7 +3278,7 @@
         <v>0.83021</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>501</v>
       </c>
@@ -3247,7 +3292,7 @@
         <v>0.84672000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>502</v>
       </c>
@@ -3261,7 +3306,7 @@
         <v>0.85836999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>503</v>
       </c>
@@ -3275,7 +3320,7 @@
         <v>0.89410999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>504</v>
       </c>
@@ -3289,7 +3334,7 @@
         <v>0.89902000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>505</v>
       </c>
@@ -3303,7 +3348,7 @@
         <v>0.90488999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>506</v>
       </c>
@@ -3317,7 +3362,7 @@
         <v>0.91022999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>507</v>
       </c>
@@ -3331,7 +3376,7 @@
         <v>0.91751000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>508</v>
       </c>
@@ -3345,7 +3390,7 @@
         <v>0.91601999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>509</v>
       </c>
@@ -3359,7 +3404,7 @@
         <v>0.91622000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>510</v>
       </c>
@@ -3373,7 +3418,7 @@
         <v>0.91542999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>511</v>
       </c>
@@ -3387,7 +3432,7 @@
         <v>0.91064000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>512</v>
       </c>
@@ -3401,7 +3446,7 @@
         <v>0.90941000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>513</v>
       </c>
@@ -3415,7 +3460,7 @@
         <v>0.90781000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>513.5</v>
       </c>
@@ -3429,7 +3474,7 @@
         <v>0.90536000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>514</v>
       </c>
@@ -3443,7 +3488,7 @@
         <v>0.90176000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>514.5</v>
       </c>
@@ -3457,7 +3502,7 @@
         <v>0.90027999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>515</v>
       </c>
@@ -3471,7 +3516,7 @@
         <v>0.90112000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>515.5</v>
       </c>
@@ -3485,7 +3530,7 @@
         <v>0.90083999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>516</v>
       </c>
@@ -3499,7 +3544,7 @@
         <v>0.90046999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>516.5</v>
       </c>
@@ -3513,7 +3558,7 @@
         <v>0.90000999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>517</v>
       </c>
@@ -3527,7 +3572,7 @@
         <v>0.90012000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>517.5</v>
       </c>
@@ -3541,7 +3586,7 @@
         <v>0.89953000000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>518</v>
       </c>
@@ -3555,7 +3600,7 @@
         <v>0.89756000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>518.5</v>
       </c>
@@ -3569,7 +3614,7 @@
         <v>0.89692000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>519</v>
       </c>
@@ -3583,7 +3628,7 @@
         <v>0.89273999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>519.5</v>
       </c>
@@ -3597,7 +3642,7 @@
         <v>0.89139000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>520</v>
       </c>
@@ -3611,7 +3656,7 @@
         <v>0.88961000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>530</v>
       </c>
@@ -3625,7 +3670,7 @@
         <v>0.88100999999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>540</v>
       </c>
@@ -3639,7 +3684,7 @@
         <v>0.86670999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>550</v>
       </c>
@@ -3653,7 +3698,7 @@
         <v>0.85370000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>560</v>
       </c>
@@ -3667,7 +3712,7 @@
         <v>0.83816999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>570</v>
       </c>
@@ -3681,7 +3726,7 @@
         <v>0.82765999999999995</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>580</v>
       </c>
@@ -3695,7 +3740,7 @@
         <v>0.81459000000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>590</v>
       </c>
@@ -3709,7 +3754,7 @@
         <v>0.80322000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>600</v>
       </c>
@@ -3723,7 +3768,7 @@
         <v>0.80212000000000006</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>700</v>
       </c>
@@ -3737,7 +3782,7 @@
         <v>0.77420999999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>800</v>
       </c>
@@ -3751,7 +3796,7 @@
         <v>0.76176999999999995</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>900</v>
       </c>
@@ -3765,7 +3810,7 @@
         <v>0.75244999999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>1000</v>
       </c>
@@ -3779,7 +3824,7 @@
         <v>0.74189000000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>1500</v>
       </c>
@@ -3793,7 +3838,7 @@
         <v>0.73053999999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>2000</v>
       </c>
@@ -3805,6 +3850,1630 @@
       </c>
       <c r="D51">
         <v>0.69059999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22640D80-2DD8-2E48-971F-6FCFC7F6D843}">
+  <dimension ref="A1:Z44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C2">
+        <v>3.851</v>
+      </c>
+      <c r="D2">
+        <v>2E-3</v>
+      </c>
+      <c r="E2">
+        <v>17.41</v>
+      </c>
+      <c r="F2">
+        <v>0.05</v>
+      </c>
+      <c r="G2">
+        <v>-167</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>0.02</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3">
+        <v>12.499000000000001</v>
+      </c>
+      <c r="B3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C3">
+        <v>3.9670000000000001</v>
+      </c>
+      <c r="D3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E3">
+        <v>20.93</v>
+      </c>
+      <c r="F3">
+        <v>0.02</v>
+      </c>
+      <c r="G3">
+        <v>-169.5</v>
+      </c>
+      <c r="H3">
+        <v>0.06</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>0.02</v>
+      </c>
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>3.9740000000000002</v>
+      </c>
+      <c r="D4">
+        <v>1E-3</v>
+      </c>
+      <c r="E4">
+        <v>25.66</v>
+      </c>
+      <c r="F4">
+        <v>0.02</v>
+      </c>
+      <c r="G4">
+        <v>-171</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5">
+        <v>17.5</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>4.0049999999999999</v>
+      </c>
+      <c r="D5">
+        <v>1E-3</v>
+      </c>
+      <c r="E5">
+        <v>31.75</v>
+      </c>
+      <c r="F5">
+        <v>0.02</v>
+      </c>
+      <c r="G5">
+        <v>-171.5</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>0.05</v>
+      </c>
+      <c r="K5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>0.01</v>
+      </c>
+      <c r="C6">
+        <v>4.0284000000000004</v>
+      </c>
+      <c r="D6">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E6">
+        <v>39.65</v>
+      </c>
+      <c r="F6">
+        <v>0.02</v>
+      </c>
+      <c r="G6">
+        <v>-171.8</v>
+      </c>
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7">
+        <v>20.25</v>
+      </c>
+      <c r="B7">
+        <v>0.01</v>
+      </c>
+      <c r="C7">
+        <v>4.0305999999999997</v>
+      </c>
+      <c r="D7">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E7">
+        <v>40.630000000000003</v>
+      </c>
+      <c r="F7">
+        <v>0.02</v>
+      </c>
+      <c r="G7">
+        <v>-171.6</v>
+      </c>
+      <c r="H7">
+        <v>0.3</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8">
+        <v>20.5</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+      <c r="C8">
+        <v>4.0324999999999998</v>
+      </c>
+      <c r="D8">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E8">
+        <v>41.56</v>
+      </c>
+      <c r="F8">
+        <v>0.03</v>
+      </c>
+      <c r="G8">
+        <v>-171.2</v>
+      </c>
+      <c r="H8">
+        <v>0.4</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>0.05</v>
+      </c>
+      <c r="S8">
+        <v>30</v>
+      </c>
+      <c r="T8">
+        <v>0.02</v>
+      </c>
+      <c r="U8">
+        <v>4.0670000000000002</v>
+      </c>
+      <c r="V8">
+        <v>1E-3</v>
+      </c>
+      <c r="W8">
+        <v>626</v>
+      </c>
+      <c r="X8">
+        <v>2</v>
+      </c>
+      <c r="Y8">
+        <v>-23</v>
+      </c>
+      <c r="Z8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9">
+        <v>20.75</v>
+      </c>
+      <c r="B9">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>4.0324999999999998</v>
+      </c>
+      <c r="D9">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E9">
+        <v>42.56</v>
+      </c>
+      <c r="F9">
+        <v>0.02</v>
+      </c>
+      <c r="G9">
+        <v>-171.3</v>
+      </c>
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>0.05</v>
+      </c>
+      <c r="S9">
+        <v>40</v>
+      </c>
+      <c r="T9">
+        <v>0.02</v>
+      </c>
+      <c r="U9">
+        <v>4.0949999999999998</v>
+      </c>
+      <c r="V9">
+        <v>1E-3</v>
+      </c>
+      <c r="W9">
+        <v>117</v>
+      </c>
+      <c r="X9">
+        <v>2</v>
+      </c>
+      <c r="Y9">
+        <v>-6.5</v>
+      </c>
+      <c r="Z9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>0.01</v>
+      </c>
+      <c r="C10">
+        <v>4.0330000000000004</v>
+      </c>
+      <c r="D10">
+        <v>1E-3</v>
+      </c>
+      <c r="E10">
+        <v>43.46</v>
+      </c>
+      <c r="F10">
+        <v>0.02</v>
+      </c>
+      <c r="G10">
+        <v>-171.3</v>
+      </c>
+      <c r="H10">
+        <v>0.4</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>0.05</v>
+      </c>
+      <c r="S10">
+        <v>50</v>
+      </c>
+      <c r="T10">
+        <v>0.02</v>
+      </c>
+      <c r="U10">
+        <v>4.1150000000000002</v>
+      </c>
+      <c r="V10">
+        <v>1E-3</v>
+      </c>
+      <c r="W10">
+        <v>86.2</v>
+      </c>
+      <c r="X10">
+        <v>0.5</v>
+      </c>
+      <c r="Y10">
+        <v>-6.3</v>
+      </c>
+      <c r="Z10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11">
+        <v>21.25</v>
+      </c>
+      <c r="B11">
+        <v>0.01</v>
+      </c>
+      <c r="C11">
+        <v>4.0359999999999996</v>
+      </c>
+      <c r="D11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E11">
+        <v>44.52</v>
+      </c>
+      <c r="F11">
+        <v>2E-3</v>
+      </c>
+      <c r="G11">
+        <v>-171.7</v>
+      </c>
+      <c r="H11">
+        <v>0.4</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>0.05</v>
+      </c>
+      <c r="S11">
+        <v>60</v>
+      </c>
+      <c r="T11">
+        <v>0.02</v>
+      </c>
+      <c r="U11">
+        <v>4.133</v>
+      </c>
+      <c r="V11">
+        <v>1E-3</v>
+      </c>
+      <c r="W11">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="X11">
+        <v>0.6</v>
+      </c>
+      <c r="Y11">
+        <v>-6.1</v>
+      </c>
+      <c r="Z11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12">
+        <v>21.5</v>
+      </c>
+      <c r="B12">
+        <v>0.01</v>
+      </c>
+      <c r="C12">
+        <v>4.0369999999999999</v>
+      </c>
+      <c r="D12">
+        <v>1E-3</v>
+      </c>
+      <c r="E12">
+        <v>45.53</v>
+      </c>
+      <c r="F12">
+        <v>0.02</v>
+      </c>
+      <c r="G12">
+        <v>-172.4</v>
+      </c>
+      <c r="H12">
+        <v>0.7</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>0.05</v>
+      </c>
+      <c r="S12">
+        <v>65</v>
+      </c>
+      <c r="T12">
+        <v>0.02</v>
+      </c>
+      <c r="U12">
+        <v>4.141</v>
+      </c>
+      <c r="V12">
+        <v>1E-3</v>
+      </c>
+      <c r="W12">
+        <v>73.3</v>
+      </c>
+      <c r="X12">
+        <v>0.5</v>
+      </c>
+      <c r="Y12">
+        <v>-5.3</v>
+      </c>
+      <c r="Z12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13">
+        <v>21.75</v>
+      </c>
+      <c r="B13">
+        <v>0.02</v>
+      </c>
+      <c r="C13">
+        <v>4.0380000000000003</v>
+      </c>
+      <c r="D13">
+        <v>2E-3</v>
+      </c>
+      <c r="E13">
+        <v>46.61</v>
+      </c>
+      <c r="F13">
+        <v>0.03</v>
+      </c>
+      <c r="G13">
+        <v>-173.1</v>
+      </c>
+      <c r="H13">
+        <v>0.6</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>0.05</v>
+      </c>
+      <c r="S13">
+        <v>70</v>
+      </c>
+      <c r="T13">
+        <v>0.02</v>
+      </c>
+      <c r="U13">
+        <v>4.1470000000000002</v>
+      </c>
+      <c r="V13">
+        <v>1E-3</v>
+      </c>
+      <c r="W13">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="X13">
+        <v>0.4</v>
+      </c>
+      <c r="Y13">
+        <v>-4.8</v>
+      </c>
+      <c r="Z13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0.01</v>
+      </c>
+      <c r="C14">
+        <v>4.04</v>
+      </c>
+      <c r="D14">
+        <v>1E-3</v>
+      </c>
+      <c r="E14">
+        <v>47.65</v>
+      </c>
+      <c r="F14">
+        <v>0.02</v>
+      </c>
+      <c r="G14">
+        <v>-173.6</v>
+      </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>0.05</v>
+      </c>
+      <c r="S14">
+        <v>75</v>
+      </c>
+      <c r="T14">
+        <v>0.02</v>
+      </c>
+      <c r="U14">
+        <v>4.1550000000000002</v>
+      </c>
+      <c r="V14">
+        <v>1E-3</v>
+      </c>
+      <c r="W14">
+        <v>69.7</v>
+      </c>
+      <c r="X14">
+        <v>0.5</v>
+      </c>
+      <c r="Y14">
+        <v>-3.9</v>
+      </c>
+      <c r="Z14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15">
+        <v>22.25</v>
+      </c>
+      <c r="B15">
+        <v>0.01</v>
+      </c>
+      <c r="C15">
+        <v>4.0410000000000004</v>
+      </c>
+      <c r="D15">
+        <v>1E-3</v>
+      </c>
+      <c r="E15">
+        <v>48.63</v>
+      </c>
+      <c r="F15">
+        <v>0.02</v>
+      </c>
+      <c r="G15">
+        <v>-173.8</v>
+      </c>
+      <c r="H15">
+        <v>0.6</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>0.05</v>
+      </c>
+      <c r="S15">
+        <v>75.25</v>
+      </c>
+      <c r="T15">
+        <v>0.02</v>
+      </c>
+      <c r="U15">
+        <v>4.1559999999999997</v>
+      </c>
+      <c r="V15">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16">
+        <v>22.5</v>
+      </c>
+      <c r="B16">
+        <v>0.01</v>
+      </c>
+      <c r="C16">
+        <v>4.0410000000000004</v>
+      </c>
+      <c r="D16">
+        <v>1E-3</v>
+      </c>
+      <c r="E16">
+        <v>49.85</v>
+      </c>
+      <c r="F16">
+        <v>0.03</v>
+      </c>
+      <c r="G16">
+        <v>-173.4</v>
+      </c>
+      <c r="H16">
+        <v>0.6</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>22.75</v>
+      </c>
+      <c r="B17">
+        <v>0.01</v>
+      </c>
+      <c r="C17">
+        <v>4.0430000000000001</v>
+      </c>
+      <c r="D17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E17">
+        <v>51.06</v>
+      </c>
+      <c r="F17">
+        <v>0.06</v>
+      </c>
+      <c r="G17">
+        <v>-173.4</v>
+      </c>
+      <c r="H17">
+        <v>0.6</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>0.01</v>
+      </c>
+      <c r="C18">
+        <v>4.0449999999999999</v>
+      </c>
+      <c r="D18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E18">
+        <v>52.24</v>
+      </c>
+      <c r="F18">
+        <v>0.02</v>
+      </c>
+      <c r="G18">
+        <v>-173.1</v>
+      </c>
+      <c r="H18">
+        <v>0.4</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>0.01</v>
+      </c>
+      <c r="C19">
+        <v>4.0490000000000004</v>
+      </c>
+      <c r="D19">
+        <v>2E-3</v>
+      </c>
+      <c r="E19">
+        <v>63.25</v>
+      </c>
+      <c r="F19">
+        <v>0.03</v>
+      </c>
+      <c r="G19">
+        <v>-172.9</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>25.25</v>
+      </c>
+      <c r="B20">
+        <v>0.01</v>
+      </c>
+      <c r="C20">
+        <v>4.05</v>
+      </c>
+      <c r="D20">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E20">
+        <v>64.75</v>
+      </c>
+      <c r="F20">
+        <v>0.03</v>
+      </c>
+      <c r="G20">
+        <v>-172.7</v>
+      </c>
+      <c r="H20">
+        <v>0.4</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>25.5</v>
+      </c>
+      <c r="B21">
+        <v>0.01</v>
+      </c>
+      <c r="C21">
+        <v>4.0490000000000004</v>
+      </c>
+      <c r="D21">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E21">
+        <v>66.349999999999994</v>
+      </c>
+      <c r="F21">
+        <v>0.06</v>
+      </c>
+      <c r="G21">
+        <v>-172.4</v>
+      </c>
+      <c r="H21">
+        <v>0.7</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>25.75</v>
+      </c>
+      <c r="B22">
+        <v>0.01</v>
+      </c>
+      <c r="C22">
+        <v>4.0510000000000002</v>
+      </c>
+      <c r="D22">
+        <v>1E-3</v>
+      </c>
+      <c r="E22">
+        <v>68.05</v>
+      </c>
+      <c r="F22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G22">
+        <v>-172.5</v>
+      </c>
+      <c r="H22">
+        <v>0.5</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>0.02</v>
+      </c>
+      <c r="C23">
+        <v>4.0510000000000002</v>
+      </c>
+      <c r="D23">
+        <v>1E-3</v>
+      </c>
+      <c r="E23">
+        <v>69.81</v>
+      </c>
+      <c r="F23">
+        <v>0.02</v>
+      </c>
+      <c r="G23">
+        <v>-172.5</v>
+      </c>
+      <c r="H23">
+        <v>0.5</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>27.5</v>
+      </c>
+      <c r="B24">
+        <v>0.02</v>
+      </c>
+      <c r="C24">
+        <v>4.0540000000000003</v>
+      </c>
+      <c r="D24">
+        <v>1E-3</v>
+      </c>
+      <c r="E24">
+        <v>80.650000000000006</v>
+      </c>
+      <c r="F24">
+        <v>0.05</v>
+      </c>
+      <c r="G24">
+        <v>-172</v>
+      </c>
+      <c r="H24">
+        <v>0.5</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>0.02</v>
+      </c>
+      <c r="C25">
+        <v>4.0679999999999996</v>
+      </c>
+      <c r="D25">
+        <v>2E-3</v>
+      </c>
+      <c r="E25">
+        <v>106.2</v>
+      </c>
+      <c r="F25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G25">
+        <v>-171.4</v>
+      </c>
+      <c r="H25">
+        <v>0.4</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="J25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>32.5</v>
+      </c>
+      <c r="B26">
+        <v>0.03</v>
+      </c>
+      <c r="C26">
+        <v>4.0789999999999997</v>
+      </c>
+      <c r="D26">
+        <v>1E-3</v>
+      </c>
+      <c r="E26">
+        <v>144.19999999999999</v>
+      </c>
+      <c r="F26">
+        <v>0.1</v>
+      </c>
+      <c r="G26">
+        <v>-170</v>
+      </c>
+      <c r="H26">
+        <v>0.3</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+      <c r="J26">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>0.02</v>
+      </c>
+      <c r="C27">
+        <v>4.0860000000000003</v>
+      </c>
+      <c r="D27">
+        <v>1E-3</v>
+      </c>
+      <c r="E27">
+        <v>205.7</v>
+      </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="G27">
+        <v>-168</v>
+      </c>
+      <c r="H27">
+        <v>0.3</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>37.5</v>
+      </c>
+      <c r="B28">
+        <v>0.02</v>
+      </c>
+      <c r="C28">
+        <v>4.0919999999999996</v>
+      </c>
+      <c r="D28">
+        <v>1E-3</v>
+      </c>
+      <c r="E28">
+        <v>323.39999999999998</v>
+      </c>
+      <c r="F28">
+        <v>0.1</v>
+      </c>
+      <c r="G28">
+        <v>-164.8</v>
+      </c>
+      <c r="H28">
+        <v>0.2</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>0.02</v>
+      </c>
+      <c r="C29">
+        <v>4.0979999999999999</v>
+      </c>
+      <c r="D29">
+        <v>1E-3</v>
+      </c>
+      <c r="E29">
+        <v>616.20000000000005</v>
+      </c>
+      <c r="F29">
+        <v>0.2</v>
+      </c>
+      <c r="G29">
+        <v>-155</v>
+      </c>
+      <c r="H29">
+        <v>0.3</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>42.5</v>
+      </c>
+      <c r="B30">
+        <v>0.03</v>
+      </c>
+      <c r="C30">
+        <v>4.101</v>
+      </c>
+      <c r="D30">
+        <v>1E-3</v>
+      </c>
+      <c r="E30">
+        <v>1658</v>
+      </c>
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+      <c r="G30">
+        <v>-108</v>
+      </c>
+      <c r="H30">
+        <v>0.3</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>42.75</v>
+      </c>
+      <c r="B31">
+        <v>0.03</v>
+      </c>
+      <c r="C31">
+        <v>4.101</v>
+      </c>
+      <c r="D31">
+        <v>1E-3</v>
+      </c>
+      <c r="E31">
+        <v>1761</v>
+      </c>
+      <c r="F31" s="8">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>-97</v>
+      </c>
+      <c r="H31">
+        <v>0.4</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>43</v>
+      </c>
+      <c r="B32">
+        <v>0.03</v>
+      </c>
+      <c r="C32">
+        <v>4.1020000000000003</v>
+      </c>
+      <c r="D32">
+        <v>1E-3</v>
+      </c>
+      <c r="E32">
+        <v>1799.5</v>
+      </c>
+      <c r="F32">
+        <v>0.5</v>
+      </c>
+      <c r="G32">
+        <v>-85.1</v>
+      </c>
+      <c r="H32">
+        <v>0.4</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>43.24</v>
+      </c>
+      <c r="B33">
+        <v>0.03</v>
+      </c>
+      <c r="C33">
+        <v>4.1020000000000003</v>
+      </c>
+      <c r="D33">
+        <v>1E-3</v>
+      </c>
+      <c r="E33">
+        <v>1760</v>
+      </c>
+      <c r="F33">
+        <v>0.5</v>
+      </c>
+      <c r="G33">
+        <v>-73.400000000000006</v>
+      </c>
+      <c r="H33">
+        <v>0.4</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>43.5</v>
+      </c>
+      <c r="B34">
+        <v>0.01</v>
+      </c>
+      <c r="C34">
+        <v>4.1040000000000001</v>
+      </c>
+      <c r="D34">
+        <v>1E-3</v>
+      </c>
+      <c r="E34">
+        <v>1664.5</v>
+      </c>
+      <c r="F34">
+        <v>0.5</v>
+      </c>
+      <c r="G34">
+        <v>-62.8</v>
+      </c>
+      <c r="H34">
+        <v>0.3</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>43.75</v>
+      </c>
+      <c r="B35">
+        <v>0.01</v>
+      </c>
+      <c r="C35">
+        <v>4.1029999999999998</v>
+      </c>
+      <c r="D35">
+        <v>1E-3</v>
+      </c>
+      <c r="E35">
+        <v>1533.5</v>
+      </c>
+      <c r="F35">
+        <v>0.5</v>
+      </c>
+      <c r="G35">
+        <v>-53.7</v>
+      </c>
+      <c r="H35">
+        <v>0.2</v>
+      </c>
+      <c r="I35">
+        <v>5</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>0.01</v>
+      </c>
+      <c r="C36">
+        <v>4.1040000000000001</v>
+      </c>
+      <c r="D36">
+        <v>1E-3</v>
+      </c>
+      <c r="E36">
+        <v>1396.5</v>
+      </c>
+      <c r="F36">
+        <v>0.5</v>
+      </c>
+      <c r="G36">
+        <v>-46.4</v>
+      </c>
+      <c r="H36">
+        <v>0.2</v>
+      </c>
+      <c r="I36">
+        <v>5</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>44.25</v>
+      </c>
+      <c r="B37">
+        <v>0.02</v>
+      </c>
+      <c r="C37">
+        <v>4.1050000000000004</v>
+      </c>
+      <c r="D37">
+        <v>1E-3</v>
+      </c>
+      <c r="E37">
+        <v>1267</v>
+      </c>
+      <c r="F37">
+        <v>0.5</v>
+      </c>
+      <c r="G37">
+        <v>-40.200000000000003</v>
+      </c>
+      <c r="H37">
+        <v>0.5</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>44.5</v>
+      </c>
+      <c r="B38">
+        <v>0.03</v>
+      </c>
+      <c r="C38">
+        <v>4.1050000000000004</v>
+      </c>
+      <c r="D38">
+        <v>1E-3</v>
+      </c>
+      <c r="E38">
+        <v>1150.2</v>
+      </c>
+      <c r="F38">
+        <v>0.5</v>
+      </c>
+      <c r="G38">
+        <v>-35.200000000000003</v>
+      </c>
+      <c r="H38">
+        <v>0.5</v>
+      </c>
+      <c r="I38">
+        <v>5</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39">
+        <v>44.75</v>
+      </c>
+      <c r="B39">
+        <v>0.03</v>
+      </c>
+      <c r="C39">
+        <v>4.1059999999999999</v>
+      </c>
+      <c r="D39">
+        <v>1E-3</v>
+      </c>
+      <c r="E39">
+        <v>1049</v>
+      </c>
+      <c r="F39">
+        <v>0.5</v>
+      </c>
+      <c r="G39">
+        <v>-31.3</v>
+      </c>
+      <c r="H39">
+        <v>0.5</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40">
+        <v>45</v>
+      </c>
+      <c r="B40">
+        <v>0.03</v>
+      </c>
+      <c r="C40">
+        <v>4.1059999999999999</v>
+      </c>
+      <c r="D40">
+        <v>1E-3</v>
+      </c>
+      <c r="E40">
+        <v>961.5</v>
+      </c>
+      <c r="F40">
+        <v>0.3</v>
+      </c>
+      <c r="G40">
+        <v>-27.8</v>
+      </c>
+      <c r="H40">
+        <v>0.4</v>
+      </c>
+      <c r="I40">
+        <v>5</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41">
+        <v>47.5</v>
+      </c>
+      <c r="B41">
+        <v>0.03</v>
+      </c>
+      <c r="C41">
+        <v>4.1109999999999998</v>
+      </c>
+      <c r="D41">
+        <v>1E-3</v>
+      </c>
+      <c r="E41">
+        <v>519.20000000000005</v>
+      </c>
+      <c r="F41">
+        <v>0.1</v>
+      </c>
+      <c r="G41">
+        <v>-12.1</v>
+      </c>
+      <c r="H41">
+        <v>0.3</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+      <c r="J41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42">
+        <v>50</v>
+      </c>
+      <c r="B42">
+        <v>0.03</v>
+      </c>
+      <c r="C42">
+        <v>4.117</v>
+      </c>
+      <c r="D42">
+        <v>1E-3</v>
+      </c>
+      <c r="E42">
+        <v>364.2</v>
+      </c>
+      <c r="F42">
+        <v>0.1</v>
+      </c>
+      <c r="G42">
+        <v>-7.1</v>
+      </c>
+      <c r="H42">
+        <v>0.2</v>
+      </c>
+      <c r="I42">
+        <v>5</v>
+      </c>
+      <c r="J42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43">
+        <v>52.5</v>
+      </c>
+      <c r="B43">
+        <v>0.03</v>
+      </c>
+      <c r="C43">
+        <v>4.1219999999999999</v>
+      </c>
+      <c r="D43">
+        <v>1E-3</v>
+      </c>
+      <c r="E43">
+        <v>287.5</v>
+      </c>
+      <c r="F43">
+        <v>0.1</v>
+      </c>
+      <c r="G43">
+        <v>-4.7</v>
+      </c>
+      <c r="H43">
+        <v>0.3</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44">
+        <v>55</v>
+      </c>
+      <c r="B44">
+        <v>0.02</v>
+      </c>
+      <c r="C44">
+        <v>4.1260000000000003</v>
+      </c>
+      <c r="D44">
+        <v>1E-3</v>
+      </c>
+      <c r="E44">
+        <v>248.3</v>
+      </c>
+      <c r="F44">
+        <v>0.1</v>
+      </c>
+      <c r="G44">
+        <v>-4</v>
+      </c>
+      <c r="H44">
+        <v>0.1</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>